<commit_message>
Added numbers to task name and subtaskname.
</commit_message>
<xml_diff>
--- a/Chandrashekhar MH/Chandrashekhar MH.xlsx
+++ b/Chandrashekhar MH/Chandrashekhar MH.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="200">
   <si>
     <t>Version</t>
   </si>
@@ -93,7 +93,10 @@
     <t>C3 Automation</t>
   </si>
   <si>
-    <t>SampleTask111</t>
+    <t>SampleTask1111</t>
+  </si>
+  <si>
+    <t>SubTask11name</t>
   </si>
   <si>
     <t>SampleTask1Desciption</t>
@@ -957,6 +960,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color rgb="FFFFC000"/>
       <name val="Calibri"/>
@@ -967,14 +978,6 @@
       <b/>
       <sz val="12"/>
       <color rgb="FFFFC000"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="9"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1890,7 +1893,7 @@
   <dimension ref="A1:Y31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1957,7 +1960,6 @@
         <v>15</v>
       </c>
       <c r="N1"/>
-      <c r="O1" s="15"/>
       <c r="S1" s="19"/>
       <c r="T1" s="19"/>
       <c r="U1"/>
@@ -1979,14 +1981,17 @@
       <c r="D2" t="s">
         <v>18</v>
       </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I2" s="17">
         <v>20</v>
@@ -1998,10 +2003,10 @@
         <v>45423</v>
       </c>
       <c r="L2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
@@ -2011,22 +2016,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I3" s="17">
         <v>20</v>
@@ -2038,10 +2043,10 @@
         <v>45423</v>
       </c>
       <c r="L3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
@@ -2051,16 +2056,16 @@
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H4" s="17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I4">
         <v>20</v>
@@ -2072,10 +2077,10 @@
         <v>45423</v>
       </c>
       <c r="L4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
@@ -2085,16 +2090,16 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" t="s">
         <v>32</v>
       </c>
-      <c r="F5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" t="s">
-        <v>31</v>
-      </c>
       <c r="H5" s="17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I5">
         <v>20</v>
@@ -2106,10 +2111,10 @@
         <v>45423</v>
       </c>
       <c r="L5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
@@ -2125,16 +2130,16 @@
         <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I6">
         <v>20</v>
@@ -2146,10 +2151,10 @@
         <v>45423</v>
       </c>
       <c r="L6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
@@ -2273,24 +2278,24 @@
   <sheetData>
     <row r="3" customFormat="1" ht="23.4" spans="4:4">
       <c r="D3" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" customFormat="1" ht="18" spans="5:5">
       <c r="E5" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" customFormat="1" ht="15.6" spans="4:7">
       <c r="D7" s="5"/>
       <c r="E7" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" customFormat="1" ht="15.6" spans="4:7">
@@ -2299,10 +2304,10 @@
         <v>3</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" customFormat="1" spans="5:7">
@@ -2310,10 +2315,10 @@
         <v>4</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" customFormat="1" spans="5:7">
@@ -2321,10 +2326,10 @@
         <v>5</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" customFormat="1" spans="5:7">
@@ -2332,10 +2337,10 @@
         <v>6</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" customFormat="1" spans="5:7">
@@ -2343,10 +2348,10 @@
         <v>7</v>
       </c>
       <c r="F12" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" customFormat="1" spans="5:7">
@@ -2354,10 +2359,10 @@
         <v>8</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" customFormat="1" spans="5:7">
@@ -2365,10 +2370,10 @@
         <v>9</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" customFormat="1" spans="5:7">
@@ -2376,10 +2381,10 @@
         <v>10</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" customFormat="1" spans="5:7">
@@ -2387,7 +2392,7 @@
         <v>11</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G16" s="11">
         <v>20</v>
@@ -2395,24 +2400,24 @@
     </row>
     <row r="17" customFormat="1" spans="5:7">
       <c r="E17" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" customFormat="1" spans="5:7">
       <c r="E18" s="9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" customFormat="1" spans="5:7">
@@ -2420,10 +2425,10 @@
         <v>14</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" customFormat="1" spans="5:7">
@@ -2431,26 +2436,26 @@
         <v>15</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" customFormat="1" spans="5:7">
       <c r="E21" s="9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" customFormat="1" ht="18" spans="3:3">
       <c r="C25" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" customFormat="1" ht="15.6" spans="2:4">
@@ -2458,7 +2463,7 @@
         <v>1</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D26" s="13"/>
     </row>
@@ -2467,7 +2472,7 @@
         <v>2</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" customFormat="1" spans="2:3">
@@ -2475,7 +2480,7 @@
         <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" customFormat="1" spans="2:3">
@@ -2483,7 +2488,7 @@
         <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" customFormat="1" spans="2:3">
@@ -2491,7 +2496,7 @@
         <v>5</v>
       </c>
       <c r="C30" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -2525,71 +2530,71 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" customFormat="1" spans="1:7">
@@ -2597,439 +2602,439 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D5" t="s">
         <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" customFormat="1" spans="1:7">
       <c r="A6" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D6" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F6" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" customFormat="1" spans="2:7">
       <c r="B7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E7" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G7" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" customFormat="1" spans="2:7">
       <c r="B8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E8" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F8" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G8" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" customFormat="1" spans="2:7">
       <c r="B9" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D9" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E9" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G9" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" customFormat="1" spans="2:7">
       <c r="B10" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C10" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D10" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E10" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F10" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G10" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" customFormat="1" spans="2:7">
       <c r="B11" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D11" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E11" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F11" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="G11" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" customFormat="1" spans="2:7">
       <c r="B12" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C12" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D12" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E12" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F12" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G12" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" customFormat="1" spans="2:6">
       <c r="B13" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D13" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E13" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F13" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" customFormat="1" spans="2:6">
       <c r="B14" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C14" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D14" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E14" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F14" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15" customFormat="1" spans="2:6">
       <c r="B15" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D15" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E15" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F15" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" customFormat="1" spans="2:6">
       <c r="B16" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E16" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F16" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="17" customFormat="1" spans="2:6">
       <c r="B17" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E17" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F17" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" customFormat="1" spans="2:6">
       <c r="B18" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E18" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F18" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" customFormat="1" spans="2:5">
       <c r="B19" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E19" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="20" customFormat="1" spans="2:5">
       <c r="B20" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E20" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="21" customFormat="1" spans="2:5">
       <c r="B21" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E21" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="22" customFormat="1" spans="2:5">
       <c r="B22" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E22" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="23" customFormat="1" spans="2:5">
       <c r="B23" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E23" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="24" customFormat="1" spans="2:5">
       <c r="B24" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E24" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="25" customFormat="1" spans="2:5">
       <c r="B25" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E25" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="26" customFormat="1" spans="2:5">
       <c r="B26" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E26" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="27" customFormat="1" spans="2:5">
       <c r="B27" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E27" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="28" customFormat="1" spans="2:5">
       <c r="B28" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E28" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="29" customFormat="1" spans="2:5">
       <c r="B29" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E29" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="30" customFormat="1" spans="2:5">
       <c r="B30" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E30" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="31" customFormat="1" spans="2:5">
       <c r="B31" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E31" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="32" customFormat="1" spans="2:5">
       <c r="B32" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E32" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="33" customFormat="1" spans="2:5">
       <c r="B33" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E33" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="34" spans="5:5">
       <c r="E34" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="35" spans="5:5">
       <c r="E35" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="36" spans="5:5">
       <c r="E36" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="37" spans="5:5">
       <c r="E37" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="38" spans="5:5">
       <c r="E38" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="39" spans="5:5">
       <c r="E39" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="40" spans="5:5">
       <c r="E40" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="41" spans="5:5">
       <c r="E41" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="42" spans="5:5">
       <c r="E42" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="43" spans="5:5">
       <c r="E43" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added extra 1 2nd time..
</commit_message>
<xml_diff>
--- a/Chandrashekhar MH/Chandrashekhar MH.xlsx
+++ b/Chandrashekhar MH/Chandrashekhar MH.xlsx
@@ -93,10 +93,10 @@
     <t>C3 Automation</t>
   </si>
   <si>
-    <t>SampleTask1111</t>
-  </si>
-  <si>
-    <t>SubTask11name</t>
+    <t>SampleTask11111</t>
+  </si>
+  <si>
+    <t>SubTask111name</t>
   </si>
   <si>
     <t>SampleTask1Desciption</t>
@@ -960,14 +960,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="9"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FFFFC000"/>
       <name val="Calibri"/>
@@ -978,6 +970,14 @@
       <b/>
       <sz val="12"/>
       <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="9"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1893,7 +1893,7 @@
   <dimension ref="A1:Y31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
added nother 1..3rd time
</commit_message>
<xml_diff>
--- a/Chandrashekhar MH/Chandrashekhar MH.xlsx
+++ b/Chandrashekhar MH/Chandrashekhar MH.xlsx
@@ -93,10 +93,10 @@
     <t>C3 Automation</t>
   </si>
   <si>
-    <t>SampleTask11111</t>
-  </si>
-  <si>
-    <t>SubTask111name</t>
+    <t>SampleTask111111</t>
+  </si>
+  <si>
+    <t>SubTask1111name</t>
   </si>
   <si>
     <t>SampleTask1Desciption</t>
@@ -960,6 +960,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color rgb="FFFFC000"/>
       <name val="Calibri"/>
@@ -970,14 +978,6 @@
       <b/>
       <sz val="12"/>
       <color rgb="FFFFC000"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="9"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1893,7 +1893,7 @@
   <dimension ref="A1:Y31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>

</xml_diff>